<commit_message>
Updated the existing file
</commit_message>
<xml_diff>
--- a/util/report_chennai.xlsx
+++ b/util/report_chennai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Syed Omar Albeez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CBB0B7-CD2A-4293-AA41-F63D96D63E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6514B2C6-B883-40E5-ACEB-4255A11C88A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17335,16 +17335,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>L3+L4+L19+L20+L57+L</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>RAJESH KUMAR K</t>
     </r>
   </si>
@@ -17907,26 +17897,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>L5+L6+L39+L40+L49+L</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>L1+L2+L15+L16+L27+L</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>FSD3004</t>
     </r>
   </si>
@@ -21134,6 +21104,15 @@
   </si>
   <si>
     <t>VENUE</t>
+  </si>
+  <si>
+    <t>L3+L4+L19+L20+L57</t>
+  </si>
+  <si>
+    <t>L5+L6+L39+L40+L49</t>
+  </si>
+  <si>
+    <t>L1+L2+L15+L16+L27</t>
   </si>
 </sst>
 </file>
@@ -21204,7 +21183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -21243,6 +21222,9 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -21700,8 +21682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A368" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A2283" workbookViewId="0">
+      <selection activeCell="F2102" sqref="F2102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -21710,31 +21692,31 @@
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
     <col min="3" max="3" width="7.21875" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1805</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1806</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1807</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1808</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1809</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1810</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1811</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1812</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -65405,20 +65387,20 @@
       <c r="D2081" s="4">
         <v>3</v>
       </c>
-      <c r="E2081" s="3" t="s">
+      <c r="E2081" s="13" t="s">
+        <v>1810</v>
+      </c>
+      <c r="F2081" s="3" t="s">
         <v>1476</v>
-      </c>
-      <c r="F2081" s="3" t="s">
-        <v>1477</v>
       </c>
       <c r="G2081" s="5"/>
     </row>
     <row r="2082" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2082" s="2" t="s">
+        <v>1477</v>
+      </c>
+      <c r="B2082" s="6" t="s">
         <v>1478</v>
-      </c>
-      <c r="B2082" s="6" t="s">
-        <v>1479</v>
       </c>
       <c r="C2082" s="3" t="s">
         <v>35</v>
@@ -65430,16 +65412,16 @@
         <v>94</v>
       </c>
       <c r="F2082" s="3" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="G2082" s="5"/>
     </row>
     <row r="2083" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2083" s="9" t="s">
+        <v>1480</v>
+      </c>
+      <c r="B2083" s="7" t="s">
         <v>1481</v>
-      </c>
-      <c r="B2083" s="7" t="s">
-        <v>1482</v>
       </c>
       <c r="C2083" s="7" t="s">
         <v>35</v>
@@ -65451,16 +65433,16 @@
         <v>13</v>
       </c>
       <c r="F2083" s="7" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="G2083" s="5"/>
     </row>
     <row r="2084" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2084" s="9" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B2084" s="7" t="s">
         <v>1484</v>
-      </c>
-      <c r="B2084" s="7" t="s">
-        <v>1485</v>
       </c>
       <c r="C2084" s="7" t="s">
         <v>35</v>
@@ -65472,16 +65454,16 @@
         <v>94</v>
       </c>
       <c r="F2084" s="7" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="G2084" s="5"/>
     </row>
     <row r="2085" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2085" s="9" t="s">
+        <v>1486</v>
+      </c>
+      <c r="B2085" s="7" t="s">
         <v>1487</v>
-      </c>
-      <c r="B2085" s="7" t="s">
-        <v>1488</v>
       </c>
       <c r="C2085" s="7" t="s">
         <v>103</v>
@@ -65493,16 +65475,16 @@
         <v>105</v>
       </c>
       <c r="F2085" s="7" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="G2085" s="5"/>
     </row>
     <row r="2086" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2086" s="2" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B2086" s="6" t="s">
         <v>1489</v>
-      </c>
-      <c r="B2086" s="6" t="s">
-        <v>1490</v>
       </c>
       <c r="C2086" s="3" t="s">
         <v>103</v>
@@ -65511,19 +65493,19 @@
         <v>3</v>
       </c>
       <c r="E2086" s="3" t="s">
+        <v>1490</v>
+      </c>
+      <c r="F2086" s="3" t="s">
         <v>1491</v>
-      </c>
-      <c r="F2086" s="3" t="s">
-        <v>1492</v>
       </c>
       <c r="G2086" s="5"/>
     </row>
     <row r="2087" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2087" s="2" t="s">
+        <v>1492</v>
+      </c>
+      <c r="B2087" s="3" t="s">
         <v>1493</v>
-      </c>
-      <c r="B2087" s="3" t="s">
-        <v>1494</v>
       </c>
       <c r="C2087" s="3" t="s">
         <v>103</v>
@@ -65532,16 +65514,16 @@
         <v>3</v>
       </c>
       <c r="E2087" s="3" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="F2087" s="3" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="G2087" s="5"/>
     </row>
     <row r="2088" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2088" s="9" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="B2088" s="7" t="s">
         <v>233</v>
@@ -65562,10 +65544,10 @@
     </row>
     <row r="2089" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2089" s="9" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B2089" s="7" t="s">
         <v>1497</v>
-      </c>
-      <c r="B2089" s="7" t="s">
-        <v>1498</v>
       </c>
       <c r="C2089" s="7" t="s">
         <v>150</v>
@@ -65577,16 +65559,16 @@
         <v>32</v>
       </c>
       <c r="F2089" s="7" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="G2089" s="5"/>
     </row>
     <row r="2090" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2090" s="9" t="s">
+        <v>1496</v>
+      </c>
+      <c r="B2090" s="7" t="s">
         <v>1497</v>
-      </c>
-      <c r="B2090" s="7" t="s">
-        <v>1498</v>
       </c>
       <c r="C2090" s="7" t="s">
         <v>710</v>
@@ -65598,16 +65580,16 @@
         <v>41</v>
       </c>
       <c r="F2090" s="7" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="G2090" s="5"/>
     </row>
     <row r="2091" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2091" s="2" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B2091" s="6" t="s">
         <v>1499</v>
-      </c>
-      <c r="B2091" s="6" t="s">
-        <v>1500</v>
       </c>
       <c r="C2091" s="3" t="s">
         <v>234</v>
@@ -65625,10 +65607,10 @@
     </row>
     <row r="2092" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2092" s="2" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B2092" s="6" t="s">
         <v>1501</v>
-      </c>
-      <c r="B2092" s="6" t="s">
-        <v>1502</v>
       </c>
       <c r="C2092" s="3" t="s">
         <v>103</v>
@@ -65637,19 +65619,19 @@
         <v>3</v>
       </c>
       <c r="E2092" s="3" t="s">
+        <v>1502</v>
+      </c>
+      <c r="F2092" s="3" t="s">
         <v>1503</v>
-      </c>
-      <c r="F2092" s="3" t="s">
-        <v>1504</v>
       </c>
       <c r="G2092" s="5"/>
     </row>
     <row r="2093" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2093" s="2" t="s">
+        <v>1500</v>
+      </c>
+      <c r="B2093" s="6" t="s">
         <v>1501</v>
-      </c>
-      <c r="B2093" s="6" t="s">
-        <v>1502</v>
       </c>
       <c r="C2093" s="3" t="s">
         <v>103</v>
@@ -65658,19 +65640,19 @@
         <v>3</v>
       </c>
       <c r="E2093" s="3" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="F2093" s="3" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="G2093" s="5"/>
     </row>
     <row r="2094" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2094" s="2" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B2094" s="3" t="s">
         <v>1506</v>
-      </c>
-      <c r="B2094" s="3" t="s">
-        <v>1507</v>
       </c>
       <c r="C2094" s="3" t="s">
         <v>150</v>
@@ -65688,10 +65670,10 @@
     </row>
     <row r="2095" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2095" s="2" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B2095" s="3" t="s">
         <v>1506</v>
-      </c>
-      <c r="B2095" s="3" t="s">
-        <v>1507</v>
       </c>
       <c r="C2095" s="3" t="s">
         <v>152</v>
@@ -65709,10 +65691,10 @@
     </row>
     <row r="2096" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2096" s="2" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B2096" s="3" t="s">
         <v>1508</v>
-      </c>
-      <c r="B2096" s="3" t="s">
-        <v>1509</v>
       </c>
       <c r="C2096" s="3" t="s">
         <v>150</v>
@@ -65730,10 +65712,10 @@
     </row>
     <row r="2097" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2097" s="2" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B2097" s="3" t="s">
         <v>1508</v>
-      </c>
-      <c r="B2097" s="3" t="s">
-        <v>1509</v>
       </c>
       <c r="C2097" s="3" t="s">
         <v>710</v>
@@ -65751,10 +65733,10 @@
     </row>
     <row r="2098" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2098" s="9" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B2098" s="7" t="s">
         <v>1510</v>
-      </c>
-      <c r="B2098" s="7" t="s">
-        <v>1511</v>
       </c>
       <c r="C2098" s="7" t="s">
         <v>150</v>
@@ -65766,16 +65748,16 @@
         <v>151</v>
       </c>
       <c r="F2098" s="7" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="G2098" s="5"/>
     </row>
     <row r="2099" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2099" s="9" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B2099" s="7" t="s">
         <v>1510</v>
-      </c>
-      <c r="B2099" s="7" t="s">
-        <v>1511</v>
       </c>
       <c r="C2099" s="7" t="s">
         <v>152</v>
@@ -65787,16 +65769,16 @@
         <v>1054</v>
       </c>
       <c r="F2099" s="7" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="G2099" s="5"/>
     </row>
     <row r="2100" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2100" s="9" t="s">
+        <v>1509</v>
+      </c>
+      <c r="B2100" s="7" t="s">
         <v>1510</v>
-      </c>
-      <c r="B2100" s="7" t="s">
-        <v>1511</v>
       </c>
       <c r="C2100" s="7" t="s">
         <v>152</v>
@@ -65805,19 +65787,19 @@
         <v>2</v>
       </c>
       <c r="E2100" s="7" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="F2100" s="7" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="G2100" s="5"/>
     </row>
     <row r="2101" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2101" s="9" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B2101" s="7" t="s">
         <v>1513</v>
-      </c>
-      <c r="B2101" s="7" t="s">
-        <v>1514</v>
       </c>
       <c r="C2101" s="7" t="s">
         <v>35</v>
@@ -65829,16 +65811,16 @@
         <v>94</v>
       </c>
       <c r="F2101" s="7" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="G2101" s="5"/>
     </row>
     <row r="2102" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2102" s="2" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B2102" s="6" t="s">
         <v>1516</v>
-      </c>
-      <c r="B2102" s="6" t="s">
-        <v>1517</v>
       </c>
       <c r="C2102" s="3" t="s">
         <v>35</v>
@@ -65850,16 +65832,16 @@
         <v>15</v>
       </c>
       <c r="F2102" s="3" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="G2102" s="5"/>
     </row>
     <row r="2103" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2103" s="2" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B2103" s="6" t="s">
         <v>1518</v>
-      </c>
-      <c r="B2103" s="6" t="s">
-        <v>1519</v>
       </c>
       <c r="C2103" s="3" t="s">
         <v>150</v>
@@ -65877,10 +65859,10 @@
     </row>
     <row r="2104" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2104" s="2" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B2104" s="6" t="s">
         <v>1518</v>
-      </c>
-      <c r="B2104" s="6" t="s">
-        <v>1519</v>
       </c>
       <c r="C2104" s="3" t="s">
         <v>710</v>
@@ -65898,11 +65880,11 @@
     </row>
     <row r="2105" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2105" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B2105" s="6" t="s">
         <v>1520</v>
       </c>
-      <c r="B2105" s="6" t="s">
-        <v>1521</v>
-      </c>
       <c r="C2105" s="3" t="s">
         <v>35</v>
       </c>
@@ -65913,16 +65895,16 @@
         <v>3</v>
       </c>
       <c r="F2105" s="3" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="G2105" s="5"/>
     </row>
     <row r="2106" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2106" s="9" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B2106" s="7" t="s">
         <v>1522</v>
-      </c>
-      <c r="B2106" s="7" t="s">
-        <v>1523</v>
       </c>
       <c r="C2106" s="7" t="s">
         <v>103</v>
@@ -65931,19 +65913,19 @@
         <v>3</v>
       </c>
       <c r="E2106" s="7" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="F2106" s="7" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="G2106" s="5"/>
     </row>
     <row r="2107" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2107" s="9" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B2107" s="7" t="s">
         <v>1522</v>
-      </c>
-      <c r="B2107" s="7" t="s">
-        <v>1523</v>
       </c>
       <c r="C2107" s="7" t="s">
         <v>103</v>
@@ -65952,19 +65934,19 @@
         <v>3</v>
       </c>
       <c r="E2107" s="7" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="F2107" s="7" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="G2107" s="5"/>
     </row>
     <row r="2108" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2108" s="2" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B2108" s="6" t="s">
         <v>1524</v>
-      </c>
-      <c r="B2108" s="6" t="s">
-        <v>1525</v>
       </c>
       <c r="C2108" s="3" t="s">
         <v>103</v>
@@ -65972,8 +65954,8 @@
       <c r="D2108" s="4">
         <v>4</v>
       </c>
-      <c r="E2108" s="3" t="s">
-        <v>1526</v>
+      <c r="E2108" s="13" t="s">
+        <v>1811</v>
       </c>
       <c r="F2108" s="3" t="s">
         <v>1464</v>
@@ -65982,10 +65964,10 @@
     </row>
     <row r="2109" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2109" s="2" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B2109" s="6" t="s">
         <v>1524</v>
-      </c>
-      <c r="B2109" s="6" t="s">
-        <v>1525</v>
       </c>
       <c r="C2109" s="3" t="s">
         <v>103</v>
@@ -65993,8 +65975,8 @@
       <c r="D2109" s="4">
         <v>4</v>
       </c>
-      <c r="E2109" s="3" t="s">
-        <v>1527</v>
+      <c r="E2109" s="13" t="s">
+        <v>1812</v>
       </c>
       <c r="F2109" s="3" t="s">
         <v>1456</v>
@@ -66003,10 +65985,10 @@
     </row>
     <row r="2110" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2110" s="2" t="s">
-        <v>1528</v>
+        <v>1525</v>
       </c>
       <c r="B2110" s="3" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
       <c r="C2110" s="3" t="s">
         <v>150</v>
@@ -66018,16 +66000,16 @@
         <v>231</v>
       </c>
       <c r="F2110" s="3" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="G2110" s="5"/>
     </row>
     <row r="2111" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2111" s="2" t="s">
-        <v>1528</v>
+        <v>1525</v>
       </c>
       <c r="B2111" s="3" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
       <c r="C2111" s="3" t="s">
         <v>152</v>
@@ -66036,19 +66018,19 @@
         <v>2</v>
       </c>
       <c r="E2111" s="3" t="s">
-        <v>1530</v>
+        <v>1527</v>
       </c>
       <c r="F2111" s="3" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="G2111" s="5"/>
     </row>
     <row r="2112" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2112" s="2" t="s">
-        <v>1528</v>
+        <v>1525</v>
       </c>
       <c r="B2112" s="3" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
       <c r="C2112" s="3" t="s">
         <v>152</v>
@@ -66060,16 +66042,16 @@
         <v>259</v>
       </c>
       <c r="F2112" s="3" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="G2112" s="5"/>
     </row>
     <row r="2113" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2113" s="9" t="s">
-        <v>1531</v>
+        <v>1528</v>
       </c>
       <c r="B2113" s="7" t="s">
-        <v>1532</v>
+        <v>1529</v>
       </c>
       <c r="C2113" s="7" t="s">
         <v>150</v>
@@ -66081,16 +66063,16 @@
         <v>189</v>
       </c>
       <c r="F2113" s="7" t="s">
-        <v>1533</v>
+        <v>1530</v>
       </c>
       <c r="G2113" s="5"/>
     </row>
     <row r="2114" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2114" s="9" t="s">
-        <v>1531</v>
+        <v>1528</v>
       </c>
       <c r="B2114" s="7" t="s">
-        <v>1532</v>
+        <v>1529</v>
       </c>
       <c r="C2114" s="7" t="s">
         <v>710</v>
@@ -66102,13 +66084,13 @@
         <v>41</v>
       </c>
       <c r="F2114" s="7" t="s">
-        <v>1533</v>
+        <v>1530</v>
       </c>
       <c r="G2114" s="5"/>
     </row>
     <row r="2115" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2115" s="2" t="s">
-        <v>1534</v>
+        <v>1531</v>
       </c>
       <c r="B2115" s="6" t="s">
         <v>1420</v>
@@ -66129,10 +66111,10 @@
     </row>
     <row r="2116" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2116" s="2" t="s">
-        <v>1535</v>
+        <v>1532</v>
       </c>
       <c r="B2116" s="6" t="s">
-        <v>1536</v>
+        <v>1533</v>
       </c>
       <c r="C2116" s="3" t="s">
         <v>35</v>
@@ -66150,10 +66132,10 @@
     </row>
     <row r="2117" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2117" s="2" t="s">
-        <v>1537</v>
+        <v>1534</v>
       </c>
       <c r="B2117" s="3" t="s">
-        <v>1538</v>
+        <v>1535</v>
       </c>
       <c r="C2117" s="3" t="s">
         <v>35</v>
@@ -66171,10 +66153,10 @@
     </row>
     <row r="2118" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2118" s="2" t="s">
-        <v>1539</v>
+        <v>1536</v>
       </c>
       <c r="B2118" s="6" t="s">
-        <v>1540</v>
+        <v>1537</v>
       </c>
       <c r="C2118" s="3" t="s">
         <v>35</v>
@@ -66186,16 +66168,16 @@
         <v>94</v>
       </c>
       <c r="F2118" s="3" t="s">
-        <v>1541</v>
+        <v>1538</v>
       </c>
       <c r="G2118" s="5"/>
     </row>
     <row r="2119" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2119" s="2" t="s">
-        <v>1542</v>
+        <v>1539</v>
       </c>
       <c r="B2119" s="3" t="s">
-        <v>1543</v>
+        <v>1540</v>
       </c>
       <c r="C2119" s="3" t="s">
         <v>35</v>
@@ -66207,16 +66189,16 @@
         <v>13</v>
       </c>
       <c r="F2119" s="6" t="s">
-        <v>1544</v>
+        <v>1541</v>
       </c>
       <c r="G2119" s="5"/>
     </row>
     <row r="2120" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2120" s="9" t="s">
-        <v>1545</v>
+        <v>1542</v>
       </c>
       <c r="B2120" s="7" t="s">
-        <v>1546</v>
+        <v>1543</v>
       </c>
       <c r="C2120" s="7" t="s">
         <v>150</v>
@@ -66234,10 +66216,10 @@
     </row>
     <row r="2121" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2121" s="9" t="s">
-        <v>1545</v>
+        <v>1542</v>
       </c>
       <c r="B2121" s="7" t="s">
-        <v>1546</v>
+        <v>1543</v>
       </c>
       <c r="C2121" s="7" t="s">
         <v>710</v>
@@ -66255,10 +66237,10 @@
     </row>
     <row r="2122" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2122" s="9" t="s">
-        <v>1547</v>
+        <v>1544</v>
       </c>
       <c r="B2122" s="7" t="s">
-        <v>1548</v>
+        <v>1545</v>
       </c>
       <c r="C2122" s="7" t="s">
         <v>35</v>
@@ -66270,16 +66252,16 @@
         <v>8</v>
       </c>
       <c r="F2122" s="7" t="s">
-        <v>1533</v>
+        <v>1530</v>
       </c>
       <c r="G2122" s="5"/>
     </row>
     <row r="2123" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2123" s="9" t="s">
-        <v>1549</v>
+        <v>1546</v>
       </c>
       <c r="B2123" s="7" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
       <c r="C2123" s="7" t="s">
         <v>150</v>
@@ -66291,16 +66273,16 @@
         <v>645</v>
       </c>
       <c r="F2123" s="7" t="s">
-        <v>1551</v>
+        <v>1548</v>
       </c>
       <c r="G2123" s="5"/>
     </row>
     <row r="2124" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2124" s="9" t="s">
-        <v>1549</v>
+        <v>1546</v>
       </c>
       <c r="B2124" s="7" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
       <c r="C2124" s="7" t="s">
         <v>710</v>
@@ -66312,16 +66294,16 @@
         <v>41</v>
       </c>
       <c r="F2124" s="7" t="s">
-        <v>1551</v>
+        <v>1548</v>
       </c>
       <c r="G2124" s="5"/>
     </row>
     <row r="2125" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2125" s="2" t="s">
-        <v>1552</v>
+        <v>1549</v>
       </c>
       <c r="B2125" s="3" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="C2125" s="3" t="s">
         <v>150</v>
@@ -66333,16 +66315,16 @@
         <v>695</v>
       </c>
       <c r="F2125" s="3" t="s">
-        <v>1554</v>
+        <v>1551</v>
       </c>
       <c r="G2125" s="5"/>
     </row>
     <row r="2126" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2126" s="2" t="s">
-        <v>1552</v>
+        <v>1549</v>
       </c>
       <c r="B2126" s="3" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="C2126" s="3" t="s">
         <v>152</v>
@@ -66354,16 +66336,16 @@
         <v>111</v>
       </c>
       <c r="F2126" s="3" t="s">
-        <v>1554</v>
+        <v>1551</v>
       </c>
       <c r="G2126" s="5"/>
     </row>
     <row r="2127" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2127" s="9" t="s">
-        <v>1555</v>
+        <v>1552</v>
       </c>
       <c r="B2127" s="7" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
       <c r="C2127" s="7" t="s">
         <v>150</v>
@@ -66381,10 +66363,10 @@
     </row>
     <row r="2128" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2128" s="9" t="s">
-        <v>1555</v>
+        <v>1552</v>
       </c>
       <c r="B2128" s="7" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
       <c r="C2128" s="7" t="s">
         <v>710</v>
@@ -66402,10 +66384,10 @@
     </row>
     <row r="2129" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2129" s="2" t="s">
-        <v>1557</v>
+        <v>1554</v>
       </c>
       <c r="B2129" s="6" t="s">
-        <v>1558</v>
+        <v>1555</v>
       </c>
       <c r="C2129" s="3" t="s">
         <v>150</v>
@@ -66417,16 +66399,16 @@
         <v>617</v>
       </c>
       <c r="F2129" s="6" t="s">
-        <v>1559</v>
+        <v>1556</v>
       </c>
       <c r="G2129" s="5"/>
     </row>
     <row r="2130" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2130" s="2" t="s">
-        <v>1557</v>
+        <v>1554</v>
       </c>
       <c r="B2130" s="6" t="s">
-        <v>1558</v>
+        <v>1555</v>
       </c>
       <c r="C2130" s="3" t="s">
         <v>710</v>
@@ -66438,16 +66420,16 @@
         <v>41</v>
       </c>
       <c r="F2130" s="6" t="s">
-        <v>1559</v>
+        <v>1556</v>
       </c>
       <c r="G2130" s="5"/>
     </row>
     <row r="2131" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2131" s="2" t="s">
-        <v>1560</v>
+        <v>1557</v>
       </c>
       <c r="B2131" s="2" t="s">
-        <v>1561</v>
+        <v>1558</v>
       </c>
       <c r="C2131" s="3" t="s">
         <v>150</v>
@@ -66465,10 +66447,10 @@
     </row>
     <row r="2132" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2132" s="2" t="s">
-        <v>1560</v>
+        <v>1557</v>
       </c>
       <c r="B2132" s="2" t="s">
-        <v>1561</v>
+        <v>1558</v>
       </c>
       <c r="C2132" s="3" t="s">
         <v>710</v>
@@ -66486,10 +66468,10 @@
     </row>
     <row r="2133" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2133" s="2" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
       <c r="B2133" s="6" t="s">
-        <v>1563</v>
+        <v>1560</v>
       </c>
       <c r="C2133" s="3" t="s">
         <v>150</v>
@@ -66501,16 +66483,16 @@
         <v>32</v>
       </c>
       <c r="F2133" s="3" t="s">
-        <v>1564</v>
+        <v>1561</v>
       </c>
       <c r="G2133" s="5"/>
     </row>
     <row r="2134" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2134" s="2" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
       <c r="B2134" s="6" t="s">
-        <v>1563</v>
+        <v>1560</v>
       </c>
       <c r="C2134" s="3" t="s">
         <v>710</v>
@@ -66522,16 +66504,16 @@
         <v>41</v>
       </c>
       <c r="F2134" s="3" t="s">
-        <v>1564</v>
+        <v>1561</v>
       </c>
       <c r="G2134" s="5"/>
     </row>
     <row r="2135" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2135" s="2" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
       <c r="B2135" s="6" t="s">
-        <v>1563</v>
+        <v>1560</v>
       </c>
       <c r="C2135" s="3" t="s">
         <v>150</v>
@@ -66543,16 +66525,16 @@
         <v>203</v>
       </c>
       <c r="F2135" s="3" t="s">
-        <v>1564</v>
+        <v>1561</v>
       </c>
       <c r="G2135" s="5"/>
     </row>
     <row r="2136" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2136" s="2" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
       <c r="B2136" s="6" t="s">
-        <v>1563</v>
+        <v>1560</v>
       </c>
       <c r="C2136" s="3" t="s">
         <v>710</v>
@@ -66564,16 +66546,16 @@
         <v>41</v>
       </c>
       <c r="F2136" s="3" t="s">
-        <v>1564</v>
+        <v>1561</v>
       </c>
       <c r="G2136" s="5"/>
     </row>
     <row r="2137" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2137" s="2" t="s">
-        <v>1565</v>
+        <v>1562</v>
       </c>
       <c r="B2137" s="6" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="C2137" s="3" t="s">
         <v>150</v>
@@ -66585,16 +66567,16 @@
         <v>98</v>
       </c>
       <c r="F2137" s="3" t="s">
-        <v>1567</v>
+        <v>1564</v>
       </c>
       <c r="G2137" s="5"/>
     </row>
     <row r="2138" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2138" s="2" t="s">
-        <v>1565</v>
+        <v>1562</v>
       </c>
       <c r="B2138" s="6" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="C2138" s="3" t="s">
         <v>710</v>
@@ -66606,16 +66588,16 @@
         <v>41</v>
       </c>
       <c r="F2138" s="3" t="s">
-        <v>1567</v>
+        <v>1564</v>
       </c>
       <c r="G2138" s="5"/>
     </row>
     <row r="2139" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2139" s="2" t="s">
-        <v>1565</v>
+        <v>1562</v>
       </c>
       <c r="B2139" s="6" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="C2139" s="3" t="s">
         <v>150</v>
@@ -66633,10 +66615,10 @@
     </row>
     <row r="2140" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2140" s="2" t="s">
-        <v>1565</v>
+        <v>1562</v>
       </c>
       <c r="B2140" s="6" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="C2140" s="3" t="s">
         <v>710</v>
@@ -66654,10 +66636,10 @@
     </row>
     <row r="2141" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2141" s="2" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="B2141" s="7" t="s">
-        <v>1569</v>
+        <v>1566</v>
       </c>
       <c r="C2141" s="3" t="s">
         <v>150</v>
@@ -66669,16 +66651,16 @@
         <v>32</v>
       </c>
       <c r="F2141" s="7" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="G2141" s="5"/>
     </row>
     <row r="2142" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2142" s="2" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="B2142" s="7" t="s">
-        <v>1569</v>
+        <v>1566</v>
       </c>
       <c r="C2142" s="3" t="s">
         <v>710</v>
@@ -66690,16 +66672,16 @@
         <v>41</v>
       </c>
       <c r="F2142" s="7" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="G2142" s="5"/>
     </row>
     <row r="2143" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2143" s="2" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="B2143" s="7" t="s">
-        <v>1569</v>
+        <v>1566</v>
       </c>
       <c r="C2143" s="3" t="s">
         <v>150</v>
@@ -66711,16 +66693,16 @@
         <v>203</v>
       </c>
       <c r="F2143" s="7" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="G2143" s="5"/>
     </row>
     <row r="2144" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2144" s="2" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="B2144" s="7" t="s">
-        <v>1569</v>
+        <v>1566</v>
       </c>
       <c r="C2144" s="3" t="s">
         <v>710</v>
@@ -66732,16 +66714,16 @@
         <v>41</v>
       </c>
       <c r="F2144" s="7" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="G2144" s="5"/>
     </row>
     <row r="2145" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2145" s="2" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
       <c r="B2145" s="3" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
       <c r="C2145" s="3" t="s">
         <v>150</v>
@@ -66753,16 +66735,16 @@
         <v>94</v>
       </c>
       <c r="F2145" s="6" t="s">
-        <v>1573</v>
+        <v>1570</v>
       </c>
       <c r="G2145" s="5"/>
     </row>
     <row r="2146" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2146" s="2" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
       <c r="B2146" s="3" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
       <c r="C2146" s="3" t="s">
         <v>710</v>
@@ -66774,16 +66756,16 @@
         <v>41</v>
       </c>
       <c r="F2146" s="6" t="s">
-        <v>1573</v>
+        <v>1570</v>
       </c>
       <c r="G2146" s="5"/>
     </row>
     <row r="2147" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2147" s="2" t="s">
-        <v>1574</v>
+        <v>1571</v>
       </c>
       <c r="B2147" s="3" t="s">
-        <v>1575</v>
+        <v>1572</v>
       </c>
       <c r="C2147" s="3" t="s">
         <v>35</v>
@@ -66795,16 +66777,16 @@
         <v>13</v>
       </c>
       <c r="F2147" s="7" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
       <c r="G2147" s="5"/>
     </row>
     <row r="2148" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2148" s="2" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="B2148" s="6" t="s">
-        <v>1578</v>
+        <v>1575</v>
       </c>
       <c r="C2148" s="3" t="s">
         <v>35</v>
@@ -66816,13 +66798,13 @@
         <v>3</v>
       </c>
       <c r="F2148" s="6" t="s">
-        <v>1544</v>
+        <v>1541</v>
       </c>
       <c r="G2148" s="5"/>
     </row>
     <row r="2149" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2149" s="2" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="B2149" s="3" t="s">
         <v>1427</v>
@@ -66837,16 +66819,16 @@
         <v>8</v>
       </c>
       <c r="F2149" s="7" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="G2149" s="5"/>
     </row>
     <row r="2150" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2150" s="9" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="B2150" s="7" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="C2150" s="7" t="s">
         <v>35</v>
@@ -66864,10 +66846,10 @@
     </row>
     <row r="2151" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2151" s="9" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="B2151" s="7" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="C2151" s="7" t="s">
         <v>35</v>
@@ -66879,16 +66861,16 @@
         <v>203</v>
       </c>
       <c r="F2151" s="7" t="s">
-        <v>1533</v>
+        <v>1530</v>
       </c>
       <c r="G2151" s="5"/>
     </row>
     <row r="2152" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2152" s="9" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="B2152" s="7" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="C2152" s="7" t="s">
         <v>35</v>
@@ -66900,13 +66882,13 @@
         <v>7</v>
       </c>
       <c r="F2152" s="7" t="s">
-        <v>1567</v>
+        <v>1564</v>
       </c>
       <c r="G2152" s="5"/>
     </row>
     <row r="2153" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2153" s="2" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="B2153" s="6" t="s">
         <v>1401</v>
@@ -66921,16 +66903,16 @@
         <v>6</v>
       </c>
       <c r="F2153" s="3" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="G2153" s="5"/>
     </row>
     <row r="2154" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2154" s="2" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="B2154" s="3" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="C2154" s="3" t="s">
         <v>35</v>
@@ -66942,16 +66924,16 @@
         <v>9</v>
       </c>
       <c r="F2154" s="6" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="G2154" s="5"/>
     </row>
     <row r="2155" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2155" s="2" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="B2155" s="3" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="C2155" s="3" t="s">
         <v>35</v>
@@ -66969,10 +66951,10 @@
     </row>
     <row r="2156" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2156" s="9" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="B2156" s="7" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="C2156" s="7" t="s">
         <v>35</v>
@@ -66990,10 +66972,10 @@
     </row>
     <row r="2157" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2157" s="2" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="B2157" s="6" t="s">
-        <v>1596</v>
+        <v>1593</v>
       </c>
       <c r="C2157" s="3" t="s">
         <v>35</v>
@@ -67011,10 +66993,10 @@
     </row>
     <row r="2158" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2158" s="2" t="s">
-        <v>1597</v>
+        <v>1594</v>
       </c>
       <c r="B2158" s="6" t="s">
-        <v>1598</v>
+        <v>1595</v>
       </c>
       <c r="C2158" s="3" t="s">
         <v>35</v>
@@ -67026,16 +67008,16 @@
         <v>14</v>
       </c>
       <c r="F2158" s="3" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="G2158" s="5"/>
     </row>
     <row r="2159" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2159" s="2" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
       <c r="B2159" s="3" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
       <c r="C2159" s="3" t="s">
         <v>35</v>
@@ -67047,16 +67029,16 @@
         <v>6</v>
       </c>
       <c r="F2159" s="3" t="s">
-        <v>1551</v>
+        <v>1548</v>
       </c>
       <c r="G2159" s="5"/>
     </row>
     <row r="2160" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2160" s="2" t="s">
-        <v>1602</v>
+        <v>1599</v>
       </c>
       <c r="B2160" s="3" t="s">
-        <v>1538</v>
+        <v>1535</v>
       </c>
       <c r="C2160" s="3" t="s">
         <v>35</v>
@@ -67068,16 +67050,16 @@
         <v>98</v>
       </c>
       <c r="F2160" s="6" t="s">
-        <v>1603</v>
+        <v>1600</v>
       </c>
       <c r="G2160" s="5"/>
     </row>
     <row r="2161" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2161" s="2" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
       <c r="B2161" s="3" t="s">
-        <v>1605</v>
+        <v>1602</v>
       </c>
       <c r="C2161" s="3" t="s">
         <v>35</v>
@@ -67089,16 +67071,16 @@
         <v>10</v>
       </c>
       <c r="F2161" s="6" t="s">
-        <v>1603</v>
+        <v>1600</v>
       </c>
       <c r="G2161" s="5"/>
     </row>
     <row r="2162" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2162" s="2" t="s">
-        <v>1606</v>
+        <v>1603</v>
       </c>
       <c r="B2162" s="3" t="s">
-        <v>1607</v>
+        <v>1604</v>
       </c>
       <c r="C2162" s="3" t="s">
         <v>35</v>
@@ -67110,16 +67092,16 @@
         <v>8</v>
       </c>
       <c r="F2162" s="6" t="s">
-        <v>1608</v>
+        <v>1605</v>
       </c>
       <c r="G2162" s="5"/>
     </row>
     <row r="2163" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2163" s="2" t="s">
-        <v>1609</v>
+        <v>1606</v>
       </c>
       <c r="B2163" s="6" t="s">
-        <v>1610</v>
+        <v>1607</v>
       </c>
       <c r="C2163" s="3" t="s">
         <v>150</v>
@@ -67137,10 +67119,10 @@
     </row>
     <row r="2164" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2164" s="2" t="s">
-        <v>1611</v>
+        <v>1608</v>
       </c>
       <c r="B2164" s="3" t="s">
-        <v>1612</v>
+        <v>1609</v>
       </c>
       <c r="C2164" s="3" t="s">
         <v>150</v>
@@ -67158,10 +67140,10 @@
     </row>
     <row r="2165" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2165" s="2" t="s">
-        <v>1613</v>
+        <v>1610</v>
       </c>
       <c r="B2165" s="3" t="s">
-        <v>1614</v>
+        <v>1611</v>
       </c>
       <c r="C2165" s="3" t="s">
         <v>35</v>
@@ -67173,16 +67155,16 @@
         <v>678</v>
       </c>
       <c r="F2165" s="6" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="G2165" s="5"/>
     </row>
     <row r="2166" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2166" s="9" t="s">
-        <v>1615</v>
+        <v>1612</v>
       </c>
       <c r="B2166" s="7" t="s">
-        <v>1616</v>
+        <v>1613</v>
       </c>
       <c r="C2166" s="7" t="s">
         <v>35</v>
@@ -67200,10 +67182,10 @@
     </row>
     <row r="2167" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2167" s="2" t="s">
-        <v>1617</v>
+        <v>1614</v>
       </c>
       <c r="B2167" s="3" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
       <c r="C2167" s="3" t="s">
         <v>35</v>
@@ -67221,7 +67203,7 @@
     </row>
     <row r="2168" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2168" s="2" t="s">
-        <v>1618</v>
+        <v>1615</v>
       </c>
       <c r="B2168" s="6" t="s">
         <v>1420</v>
@@ -67242,10 +67224,10 @@
     </row>
     <row r="2169" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2169" s="2" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="B2169" s="6" t="s">
-        <v>1620</v>
+        <v>1617</v>
       </c>
       <c r="C2169" s="3" t="s">
         <v>150</v>
@@ -67257,16 +67239,16 @@
         <v>13</v>
       </c>
       <c r="F2169" s="3" t="s">
-        <v>1621</v>
+        <v>1618</v>
       </c>
       <c r="G2169" s="5"/>
     </row>
     <row r="2170" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2170" s="2" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="B2170" s="6" t="s">
-        <v>1620</v>
+        <v>1617</v>
       </c>
       <c r="C2170" s="3" t="s">
         <v>152</v>
@@ -67278,16 +67260,16 @@
         <v>116</v>
       </c>
       <c r="F2170" s="3" t="s">
-        <v>1621</v>
+        <v>1618</v>
       </c>
       <c r="G2170" s="5"/>
     </row>
     <row r="2171" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2171" s="2" t="s">
-        <v>1622</v>
+        <v>1619</v>
       </c>
       <c r="B2171" s="6" t="s">
-        <v>1623</v>
+        <v>1620</v>
       </c>
       <c r="C2171" s="3" t="s">
         <v>35</v>
@@ -67305,10 +67287,10 @@
     </row>
     <row r="2172" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2172" s="2" t="s">
-        <v>1624</v>
+        <v>1621</v>
       </c>
       <c r="B2172" s="6" t="s">
-        <v>1558</v>
+        <v>1555</v>
       </c>
       <c r="C2172" s="3" t="s">
         <v>35</v>
@@ -67320,16 +67302,16 @@
         <v>1227</v>
       </c>
       <c r="F2172" s="6" t="s">
-        <v>1559</v>
+        <v>1556</v>
       </c>
       <c r="G2172" s="5"/>
     </row>
     <row r="2173" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2173" s="9" t="s">
-        <v>1625</v>
+        <v>1622</v>
       </c>
       <c r="B2173" s="7" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
       <c r="C2173" s="7" t="s">
         <v>35</v>
@@ -67341,16 +67323,16 @@
         <v>70</v>
       </c>
       <c r="F2173" s="7" t="s">
-        <v>1621</v>
+        <v>1618</v>
       </c>
       <c r="G2173" s="5"/>
     </row>
     <row r="2174" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2174" s="9" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="B2174" s="7" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
       <c r="C2174" s="7" t="s">
         <v>35</v>
@@ -67368,10 +67350,10 @@
     </row>
     <row r="2175" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2175" s="2" t="s">
-        <v>1629</v>
+        <v>1626</v>
       </c>
       <c r="B2175" s="6" t="s">
-        <v>1630</v>
+        <v>1627</v>
       </c>
       <c r="C2175" s="3" t="s">
         <v>35</v>
@@ -67383,16 +67365,16 @@
         <v>76</v>
       </c>
       <c r="F2175" s="3" t="s">
-        <v>1621</v>
+        <v>1618</v>
       </c>
       <c r="G2175" s="5"/>
     </row>
     <row r="2176" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2176" s="2" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="B2176" s="3" t="s">
-        <v>1632</v>
+        <v>1629</v>
       </c>
       <c r="C2176" s="3" t="s">
         <v>35</v>
@@ -67404,16 +67386,16 @@
         <v>133</v>
       </c>
       <c r="F2176" s="3" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="G2176" s="5"/>
     </row>
     <row r="2177" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2177" s="2" t="s">
-        <v>1633</v>
+        <v>1630</v>
       </c>
       <c r="B2177" s="6" t="s">
-        <v>1634</v>
+        <v>1631</v>
       </c>
       <c r="C2177" s="3" t="s">
         <v>35</v>
@@ -67425,16 +67407,16 @@
         <v>64</v>
       </c>
       <c r="F2177" s="3" t="s">
-        <v>1635</v>
+        <v>1632</v>
       </c>
       <c r="G2177" s="5"/>
     </row>
     <row r="2178" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2178" s="2" t="s">
-        <v>1636</v>
+        <v>1633</v>
       </c>
       <c r="B2178" s="3" t="s">
-        <v>1637</v>
+        <v>1634</v>
       </c>
       <c r="C2178" s="3" t="s">
         <v>35</v>
@@ -67446,16 +67428,16 @@
         <v>70</v>
       </c>
       <c r="F2178" s="3" t="s">
-        <v>1554</v>
+        <v>1551</v>
       </c>
       <c r="G2178" s="5"/>
     </row>
     <row r="2179" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2179" s="9" t="s">
-        <v>1638</v>
+        <v>1635</v>
       </c>
       <c r="B2179" s="7" t="s">
-        <v>1639</v>
+        <v>1636</v>
       </c>
       <c r="C2179" s="7" t="s">
         <v>35</v>
@@ -67473,10 +67455,10 @@
     </row>
     <row r="2180" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2180" s="2" t="s">
-        <v>1640</v>
+        <v>1637</v>
       </c>
       <c r="B2180" s="3" t="s">
-        <v>1575</v>
+        <v>1572</v>
       </c>
       <c r="C2180" s="3" t="s">
         <v>35</v>
@@ -67488,16 +67470,16 @@
         <v>82</v>
       </c>
       <c r="F2180" s="7" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
       <c r="G2180" s="5"/>
     </row>
     <row r="2181" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2181" s="2" t="s">
-        <v>1641</v>
+        <v>1638</v>
       </c>
       <c r="B2181" s="3" t="s">
-        <v>1642</v>
+        <v>1639</v>
       </c>
       <c r="C2181" s="3" t="s">
         <v>150</v>
@@ -67506,7 +67488,7 @@
         <v>3</v>
       </c>
       <c r="E2181" s="3" t="s">
-        <v>1643</v>
+        <v>1640</v>
       </c>
       <c r="F2181" s="6" t="s">
         <v>47</v>
@@ -67515,10 +67497,10 @@
     </row>
     <row r="2182" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2182" s="2" t="s">
-        <v>1641</v>
+        <v>1638</v>
       </c>
       <c r="B2182" s="3" t="s">
-        <v>1642</v>
+        <v>1639</v>
       </c>
       <c r="C2182" s="3" t="s">
         <v>710</v>
@@ -67536,31 +67518,31 @@
     </row>
     <row r="2183" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2183" s="2" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B2183" s="7" t="s">
+        <v>1642</v>
+      </c>
+      <c r="C2183" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2183" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2183" s="3" t="s">
+        <v>1643</v>
+      </c>
+      <c r="F2183" s="7" t="s">
         <v>1644</v>
-      </c>
-      <c r="B2183" s="7" t="s">
-        <v>1645</v>
-      </c>
-      <c r="C2183" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2183" s="4">
-        <v>3</v>
-      </c>
-      <c r="E2183" s="3" t="s">
-        <v>1646</v>
-      </c>
-      <c r="F2183" s="7" t="s">
-        <v>1647</v>
       </c>
       <c r="G2183" s="5"/>
     </row>
     <row r="2184" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2184" s="2" t="s">
-        <v>1648</v>
+        <v>1645</v>
       </c>
       <c r="B2184" s="7" t="s">
-        <v>1649</v>
+        <v>1646</v>
       </c>
       <c r="C2184" s="3" t="s">
         <v>103</v>
@@ -67569,7 +67551,7 @@
         <v>2</v>
       </c>
       <c r="E2184" s="3" t="s">
-        <v>1650</v>
+        <v>1647</v>
       </c>
       <c r="F2184" s="3" t="s">
         <v>50</v>
@@ -67578,10 +67560,10 @@
     </row>
     <row r="2185" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2185" s="2" t="s">
-        <v>1651</v>
+        <v>1648</v>
       </c>
       <c r="B2185" s="3" t="s">
-        <v>1652</v>
+        <v>1649</v>
       </c>
       <c r="C2185" s="3" t="s">
         <v>150</v>
@@ -67590,7 +67572,7 @@
         <v>3</v>
       </c>
       <c r="E2185" s="3" t="s">
-        <v>1653</v>
+        <v>1650</v>
       </c>
       <c r="F2185" s="3" t="s">
         <v>44</v>
@@ -67599,10 +67581,10 @@
     </row>
     <row r="2186" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2186" s="2" t="s">
-        <v>1651</v>
+        <v>1648</v>
       </c>
       <c r="B2186" s="3" t="s">
-        <v>1652</v>
+        <v>1649</v>
       </c>
       <c r="C2186" s="3" t="s">
         <v>710</v>
@@ -67620,10 +67602,10 @@
     </row>
     <row r="2187" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2187" s="2" t="s">
-        <v>1654</v>
+        <v>1651</v>
       </c>
       <c r="B2187" s="3" t="s">
-        <v>1655</v>
+        <v>1652</v>
       </c>
       <c r="C2187" s="3" t="s">
         <v>35</v>
@@ -67632,7 +67614,7 @@
         <v>4</v>
       </c>
       <c r="E2187" s="3" t="s">
-        <v>1656</v>
+        <v>1653</v>
       </c>
       <c r="F2187" s="3" t="s">
         <v>52</v>
@@ -67641,10 +67623,10 @@
     </row>
     <row r="2188" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2188" s="2" t="s">
-        <v>1657</v>
+        <v>1654</v>
       </c>
       <c r="B2188" s="6" t="s">
-        <v>1658</v>
+        <v>1655</v>
       </c>
       <c r="C2188" s="3" t="s">
         <v>103</v>
@@ -67653,7 +67635,7 @@
         <v>2</v>
       </c>
       <c r="E2188" s="3" t="s">
-        <v>1659</v>
+        <v>1656</v>
       </c>
       <c r="F2188" s="6" t="s">
         <v>54</v>
@@ -67662,10 +67644,10 @@
     </row>
     <row r="2189" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2189" s="2" t="s">
-        <v>1660</v>
+        <v>1657</v>
       </c>
       <c r="B2189" s="3" t="s">
-        <v>1661</v>
+        <v>1658</v>
       </c>
       <c r="C2189" s="3" t="s">
         <v>35</v>
@@ -67674,19 +67656,19 @@
         <v>4</v>
       </c>
       <c r="E2189" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2189" s="3" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="G2189" s="5"/>
     </row>
     <row r="2190" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2190" s="2" t="s">
-        <v>1660</v>
+        <v>1657</v>
       </c>
       <c r="B2190" s="3" t="s">
-        <v>1661</v>
+        <v>1658</v>
       </c>
       <c r="C2190" s="3" t="s">
         <v>35</v>
@@ -67695,19 +67677,19 @@
         <v>4</v>
       </c>
       <c r="E2190" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2190" s="6" t="s">
-        <v>1664</v>
+        <v>1661</v>
       </c>
       <c r="G2190" s="5"/>
     </row>
     <row r="2191" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2191" s="2" t="s">
-        <v>1660</v>
+        <v>1657</v>
       </c>
       <c r="B2191" s="3" t="s">
-        <v>1661</v>
+        <v>1658</v>
       </c>
       <c r="C2191" s="3" t="s">
         <v>35</v>
@@ -67716,19 +67698,19 @@
         <v>4</v>
       </c>
       <c r="E2191" s="3" t="s">
+        <v>1659</v>
+      </c>
+      <c r="F2191" s="3" t="s">
         <v>1662</v>
-      </c>
-      <c r="F2191" s="3" t="s">
-        <v>1665</v>
       </c>
       <c r="G2191" s="5"/>
     </row>
     <row r="2192" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2192" s="2" t="s">
-        <v>1660</v>
+        <v>1657</v>
       </c>
       <c r="B2192" s="3" t="s">
-        <v>1661</v>
+        <v>1658</v>
       </c>
       <c r="C2192" s="3" t="s">
         <v>35</v>
@@ -67737,7 +67719,7 @@
         <v>4</v>
       </c>
       <c r="E2192" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2192" s="3" t="s">
         <v>1444</v>
@@ -67746,10 +67728,10 @@
     </row>
     <row r="2193" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2193" s="9" t="s">
-        <v>1666</v>
+        <v>1663</v>
       </c>
       <c r="B2193" s="7" t="s">
-        <v>1667</v>
+        <v>1664</v>
       </c>
       <c r="C2193" s="7" t="s">
         <v>35</v>
@@ -67758,7 +67740,7 @@
         <v>4</v>
       </c>
       <c r="E2193" s="7" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2193" s="7" t="s">
         <v>1444</v>
@@ -67767,10 +67749,10 @@
     </row>
     <row r="2194" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2194" s="9" t="s">
-        <v>1669</v>
+        <v>1666</v>
       </c>
       <c r="B2194" s="7" t="s">
-        <v>1670</v>
+        <v>1667</v>
       </c>
       <c r="C2194" s="7" t="s">
         <v>35</v>
@@ -67779,19 +67761,19 @@
         <v>4</v>
       </c>
       <c r="E2194" s="7" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2194" s="7" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="G2194" s="5"/>
     </row>
     <row r="2195" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2195" s="2" t="s">
-        <v>1672</v>
+        <v>1669</v>
       </c>
       <c r="B2195" s="3" t="s">
-        <v>1673</v>
+        <v>1670</v>
       </c>
       <c r="C2195" s="3" t="s">
         <v>35</v>
@@ -67800,19 +67782,19 @@
         <v>4</v>
       </c>
       <c r="E2195" s="3" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2195" s="6" t="s">
-        <v>1675</v>
+        <v>1672</v>
       </c>
       <c r="G2195" s="5"/>
     </row>
     <row r="2196" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2196" s="2" t="s">
-        <v>1676</v>
+        <v>1673</v>
       </c>
       <c r="B2196" s="3" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="C2196" s="3" t="s">
         <v>35</v>
@@ -67821,19 +67803,19 @@
         <v>4</v>
       </c>
       <c r="E2196" s="3" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2196" s="3" t="s">
-        <v>1678</v>
+        <v>1675</v>
       </c>
       <c r="G2196" s="5"/>
     </row>
     <row r="2197" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2197" s="2" t="s">
-        <v>1679</v>
+        <v>1676</v>
       </c>
       <c r="B2197" s="3" t="s">
-        <v>1680</v>
+        <v>1677</v>
       </c>
       <c r="C2197" s="3" t="s">
         <v>35</v>
@@ -67842,19 +67824,19 @@
         <v>4</v>
       </c>
       <c r="E2197" s="3" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2197" s="3" t="s">
-        <v>1681</v>
+        <v>1678</v>
       </c>
       <c r="G2197" s="5"/>
     </row>
     <row r="2198" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2198" s="2" t="s">
-        <v>1682</v>
+        <v>1679</v>
       </c>
       <c r="B2198" s="3" t="s">
-        <v>1683</v>
+        <v>1680</v>
       </c>
       <c r="C2198" s="3" t="s">
         <v>35</v>
@@ -67863,19 +67845,19 @@
         <v>4</v>
       </c>
       <c r="E2198" s="3" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2198" s="3" t="s">
-        <v>1684</v>
+        <v>1681</v>
       </c>
       <c r="G2198" s="5"/>
     </row>
     <row r="2199" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2199" s="9" t="s">
-        <v>1685</v>
+        <v>1682</v>
       </c>
       <c r="B2199" s="7" t="s">
-        <v>1686</v>
+        <v>1683</v>
       </c>
       <c r="C2199" s="7" t="s">
         <v>35</v>
@@ -67884,7 +67866,7 @@
         <v>4</v>
       </c>
       <c r="E2199" s="7" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2199" s="7" t="s">
         <v>1271</v>
@@ -67893,10 +67875,10 @@
     </row>
     <row r="2200" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2200" s="9" t="s">
-        <v>1687</v>
+        <v>1684</v>
       </c>
       <c r="B2200" s="7" t="s">
-        <v>1688</v>
+        <v>1685</v>
       </c>
       <c r="C2200" s="7" t="s">
         <v>35</v>
@@ -67905,19 +67887,19 @@
         <v>4</v>
       </c>
       <c r="E2200" s="7" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2200" s="7" t="s">
-        <v>1689</v>
+        <v>1686</v>
       </c>
       <c r="G2200" s="5"/>
     </row>
     <row r="2201" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2201" s="2" t="s">
-        <v>1690</v>
+        <v>1687</v>
       </c>
       <c r="B2201" s="6" t="s">
-        <v>1691</v>
+        <v>1688</v>
       </c>
       <c r="C2201" s="3" t="s">
         <v>35</v>
@@ -67926,19 +67908,19 @@
         <v>4</v>
       </c>
       <c r="E2201" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2201" s="3" t="s">
-        <v>1692</v>
+        <v>1689</v>
       </c>
       <c r="G2201" s="5"/>
     </row>
     <row r="2202" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2202" s="2" t="s">
-        <v>1693</v>
+        <v>1690</v>
       </c>
       <c r="B2202" s="6" t="s">
-        <v>1694</v>
+        <v>1691</v>
       </c>
       <c r="C2202" s="3" t="s">
         <v>35</v>
@@ -67947,19 +67929,19 @@
         <v>4</v>
       </c>
       <c r="E2202" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2202" s="3" t="s">
-        <v>1695</v>
+        <v>1692</v>
       </c>
       <c r="G2202" s="5"/>
     </row>
     <row r="2203" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2203" s="2" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
       <c r="B2203" s="3" t="s">
-        <v>1697</v>
+        <v>1694</v>
       </c>
       <c r="C2203" s="3" t="s">
         <v>35</v>
@@ -67968,19 +67950,19 @@
         <v>4</v>
       </c>
       <c r="E2203" s="3" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2203" s="6" t="s">
-        <v>1699</v>
+        <v>1696</v>
       </c>
       <c r="G2203" s="5"/>
     </row>
     <row r="2204" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2204" s="2" t="s">
-        <v>1700</v>
+        <v>1697</v>
       </c>
       <c r="B2204" s="6" t="s">
-        <v>1701</v>
+        <v>1698</v>
       </c>
       <c r="C2204" s="3" t="s">
         <v>35</v>
@@ -67989,7 +67971,7 @@
         <v>4</v>
       </c>
       <c r="E2204" s="3" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2204" s="3" t="s">
         <v>1443</v>
@@ -67998,10 +67980,10 @@
     </row>
     <row r="2205" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2205" s="2" t="s">
-        <v>1702</v>
+        <v>1699</v>
       </c>
       <c r="B2205" s="3" t="s">
-        <v>1703</v>
+        <v>1700</v>
       </c>
       <c r="C2205" s="3" t="s">
         <v>35</v>
@@ -68010,19 +67992,19 @@
         <v>4</v>
       </c>
       <c r="E2205" s="3" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2205" s="3" t="s">
-        <v>1681</v>
+        <v>1678</v>
       </c>
       <c r="G2205" s="5"/>
     </row>
     <row r="2206" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2206" s="9" t="s">
-        <v>1704</v>
+        <v>1701</v>
       </c>
       <c r="B2206" s="7" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="C2206" s="7" t="s">
         <v>35</v>
@@ -68031,19 +68013,19 @@
         <v>4</v>
       </c>
       <c r="E2206" s="7" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2206" s="7" t="s">
-        <v>1707</v>
+        <v>1704</v>
       </c>
       <c r="G2206" s="5"/>
     </row>
     <row r="2207" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2207" s="9" t="s">
-        <v>1704</v>
+        <v>1701</v>
       </c>
       <c r="B2207" s="7" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="C2207" s="7" t="s">
         <v>35</v>
@@ -68052,19 +68034,19 @@
         <v>4</v>
       </c>
       <c r="E2207" s="7" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2207" s="7" t="s">
-        <v>1692</v>
+        <v>1689</v>
       </c>
       <c r="G2207" s="5"/>
     </row>
     <row r="2208" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2208" s="2" t="s">
-        <v>1704</v>
+        <v>1701</v>
       </c>
       <c r="B2208" s="3" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="C2208" s="3" t="s">
         <v>35</v>
@@ -68073,19 +68055,19 @@
         <v>4</v>
       </c>
       <c r="E2208" s="3" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2208" s="6" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="G2208" s="5"/>
     </row>
     <row r="2209" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2209" s="2" t="s">
-        <v>1704</v>
+        <v>1701</v>
       </c>
       <c r="B2209" s="3" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="C2209" s="3" t="s">
         <v>35</v>
@@ -68094,19 +68076,19 @@
         <v>4</v>
       </c>
       <c r="E2209" s="3" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2209" s="6" t="s">
-        <v>1699</v>
+        <v>1696</v>
       </c>
       <c r="G2209" s="5"/>
     </row>
     <row r="2210" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2210" s="2" t="s">
-        <v>1709</v>
+        <v>1706</v>
       </c>
       <c r="B2210" s="3" t="s">
-        <v>1710</v>
+        <v>1707</v>
       </c>
       <c r="C2210" s="3" t="s">
         <v>35</v>
@@ -68115,7 +68097,7 @@
         <v>4</v>
       </c>
       <c r="E2210" s="3" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2210" s="3" t="s">
         <v>1441</v>
@@ -68124,10 +68106,10 @@
     </row>
     <row r="2211" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2211" s="9" t="s">
-        <v>1711</v>
+        <v>1708</v>
       </c>
       <c r="B2211" s="7" t="s">
-        <v>1712</v>
+        <v>1709</v>
       </c>
       <c r="C2211" s="7" t="s">
         <v>35</v>
@@ -68136,19 +68118,19 @@
         <v>4</v>
       </c>
       <c r="E2211" s="7" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2211" s="7" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
       <c r="G2211" s="5"/>
     </row>
     <row r="2212" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2212" s="2" t="s">
-        <v>1711</v>
+        <v>1708</v>
       </c>
       <c r="B2212" s="3" t="s">
-        <v>1712</v>
+        <v>1709</v>
       </c>
       <c r="C2212" s="3" t="s">
         <v>35</v>
@@ -68157,19 +68139,19 @@
         <v>4</v>
       </c>
       <c r="E2212" s="3" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2212" s="3" t="s">
-        <v>1714</v>
+        <v>1711</v>
       </c>
       <c r="G2212" s="5"/>
     </row>
     <row r="2213" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2213" s="9" t="s">
-        <v>1711</v>
+        <v>1708</v>
       </c>
       <c r="B2213" s="7" t="s">
-        <v>1712</v>
+        <v>1709</v>
       </c>
       <c r="C2213" s="7" t="s">
         <v>35</v>
@@ -68178,19 +68160,19 @@
         <v>4</v>
       </c>
       <c r="E2213" s="7" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2213" s="7" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="G2213" s="5"/>
     </row>
     <row r="2214" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2214" s="9" t="s">
-        <v>1711</v>
+        <v>1708</v>
       </c>
       <c r="B2214" s="7" t="s">
-        <v>1712</v>
+        <v>1709</v>
       </c>
       <c r="C2214" s="7" t="s">
         <v>35</v>
@@ -68199,19 +68181,19 @@
         <v>4</v>
       </c>
       <c r="E2214" s="7" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2214" s="7" t="s">
-        <v>1716</v>
+        <v>1713</v>
       </c>
       <c r="G2214" s="5"/>
     </row>
     <row r="2215" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2215" s="9" t="s">
-        <v>1717</v>
+        <v>1714</v>
       </c>
       <c r="B2215" s="7" t="s">
-        <v>1718</v>
+        <v>1715</v>
       </c>
       <c r="C2215" s="7" t="s">
         <v>35</v>
@@ -68220,19 +68202,19 @@
         <v>4</v>
       </c>
       <c r="E2215" s="7" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2215" s="7" t="s">
-        <v>1719</v>
+        <v>1716</v>
       </c>
       <c r="G2215" s="5"/>
     </row>
     <row r="2216" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2216" s="2" t="s">
-        <v>1717</v>
+        <v>1714</v>
       </c>
       <c r="B2216" s="3" t="s">
-        <v>1718</v>
+        <v>1715</v>
       </c>
       <c r="C2216" s="3" t="s">
         <v>35</v>
@@ -68241,19 +68223,19 @@
         <v>4</v>
       </c>
       <c r="E2216" s="3" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2216" s="6" t="s">
-        <v>1720</v>
+        <v>1717</v>
       </c>
       <c r="G2216" s="5"/>
     </row>
     <row r="2217" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2217" s="9" t="s">
-        <v>1717</v>
+        <v>1714</v>
       </c>
       <c r="B2217" s="7" t="s">
-        <v>1718</v>
+        <v>1715</v>
       </c>
       <c r="C2217" s="7" t="s">
         <v>35</v>
@@ -68262,19 +68244,19 @@
         <v>4</v>
       </c>
       <c r="E2217" s="7" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2217" s="7" t="s">
-        <v>1721</v>
+        <v>1718</v>
       </c>
       <c r="G2217" s="5"/>
     </row>
     <row r="2218" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2218" s="9" t="s">
-        <v>1717</v>
+        <v>1714</v>
       </c>
       <c r="B2218" s="7" t="s">
-        <v>1718</v>
+        <v>1715</v>
       </c>
       <c r="C2218" s="7" t="s">
         <v>35</v>
@@ -68283,19 +68265,19 @@
         <v>4</v>
       </c>
       <c r="E2218" s="7" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2218" s="7" t="s">
-        <v>1722</v>
+        <v>1719</v>
       </c>
       <c r="G2218" s="5"/>
     </row>
     <row r="2219" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2219" s="2" t="s">
-        <v>1723</v>
+        <v>1720</v>
       </c>
       <c r="B2219" s="3" t="s">
-        <v>1724</v>
+        <v>1721</v>
       </c>
       <c r="C2219" s="3" t="s">
         <v>35</v>
@@ -68304,19 +68286,19 @@
         <v>4</v>
       </c>
       <c r="E2219" s="3" t="s">
-        <v>1725</v>
+        <v>1722</v>
       </c>
       <c r="F2219" s="6" t="s">
-        <v>1726</v>
+        <v>1723</v>
       </c>
       <c r="G2219" s="5"/>
     </row>
     <row r="2220" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2220" s="9" t="s">
-        <v>1723</v>
+        <v>1720</v>
       </c>
       <c r="B2220" s="7" t="s">
-        <v>1724</v>
+        <v>1721</v>
       </c>
       <c r="C2220" s="7" t="s">
         <v>35</v>
@@ -68325,19 +68307,19 @@
         <v>4</v>
       </c>
       <c r="E2220" s="7" t="s">
-        <v>1725</v>
+        <v>1722</v>
       </c>
       <c r="F2220" s="7" t="s">
-        <v>1727</v>
+        <v>1724</v>
       </c>
       <c r="G2220" s="5"/>
     </row>
     <row r="2221" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2221" s="9" t="s">
-        <v>1723</v>
+        <v>1720</v>
       </c>
       <c r="B2221" s="7" t="s">
-        <v>1724</v>
+        <v>1721</v>
       </c>
       <c r="C2221" s="7" t="s">
         <v>35</v>
@@ -68346,19 +68328,19 @@
         <v>4</v>
       </c>
       <c r="E2221" s="7" t="s">
+        <v>1722</v>
+      </c>
+      <c r="F2221" s="7" t="s">
         <v>1725</v>
-      </c>
-      <c r="F2221" s="7" t="s">
-        <v>1728</v>
       </c>
       <c r="G2221" s="5"/>
     </row>
     <row r="2222" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2222" s="9" t="s">
-        <v>1723</v>
+        <v>1720</v>
       </c>
       <c r="B2222" s="7" t="s">
-        <v>1724</v>
+        <v>1721</v>
       </c>
       <c r="C2222" s="7" t="s">
         <v>35</v>
@@ -68367,19 +68349,19 @@
         <v>4</v>
       </c>
       <c r="E2222" s="7" t="s">
-        <v>1725</v>
+        <v>1722</v>
       </c>
       <c r="F2222" s="7" t="s">
-        <v>1729</v>
+        <v>1726</v>
       </c>
       <c r="G2222" s="5"/>
     </row>
     <row r="2223" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2223" s="2" t="s">
-        <v>1730</v>
+        <v>1727</v>
       </c>
       <c r="B2223" s="3" t="s">
-        <v>1731</v>
+        <v>1728</v>
       </c>
       <c r="C2223" s="3" t="s">
         <v>35</v>
@@ -68388,19 +68370,19 @@
         <v>4</v>
       </c>
       <c r="E2223" s="3" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2223" s="6" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="G2223" s="5"/>
     </row>
     <row r="2224" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2224" s="2" t="s">
-        <v>1730</v>
+        <v>1727</v>
       </c>
       <c r="B2224" s="3" t="s">
-        <v>1731</v>
+        <v>1728</v>
       </c>
       <c r="C2224" s="3" t="s">
         <v>35</v>
@@ -68409,19 +68391,19 @@
         <v>4</v>
       </c>
       <c r="E2224" s="3" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2224" s="6" t="s">
-        <v>1732</v>
+        <v>1729</v>
       </c>
       <c r="G2224" s="5"/>
     </row>
     <row r="2225" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2225" s="2" t="s">
-        <v>1730</v>
+        <v>1727</v>
       </c>
       <c r="B2225" s="3" t="s">
-        <v>1731</v>
+        <v>1728</v>
       </c>
       <c r="C2225" s="3" t="s">
         <v>35</v>
@@ -68430,19 +68412,19 @@
         <v>4</v>
       </c>
       <c r="E2225" s="3" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2225" s="6" t="s">
-        <v>1733</v>
+        <v>1730</v>
       </c>
       <c r="G2225" s="5"/>
     </row>
     <row r="2226" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2226" s="9" t="s">
-        <v>1730</v>
+        <v>1727</v>
       </c>
       <c r="B2226" s="7" t="s">
-        <v>1731</v>
+        <v>1728</v>
       </c>
       <c r="C2226" s="7" t="s">
         <v>35</v>
@@ -68451,19 +68433,19 @@
         <v>4</v>
       </c>
       <c r="E2226" s="7" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2226" s="7" t="s">
-        <v>1734</v>
+        <v>1731</v>
       </c>
       <c r="G2226" s="5"/>
     </row>
     <row r="2227" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2227" s="2" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="B2227" s="3" t="s">
-        <v>1736</v>
+        <v>1733</v>
       </c>
       <c r="C2227" s="3" t="s">
         <v>35</v>
@@ -68472,19 +68454,19 @@
         <v>4</v>
       </c>
       <c r="E2227" s="3" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2227" s="3" t="s">
-        <v>1681</v>
+        <v>1678</v>
       </c>
       <c r="G2227" s="5"/>
     </row>
     <row r="2228" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2228" s="2" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="B2228" s="3" t="s">
-        <v>1736</v>
+        <v>1733</v>
       </c>
       <c r="C2228" s="3" t="s">
         <v>35</v>
@@ -68493,19 +68475,19 @@
         <v>4</v>
       </c>
       <c r="E2228" s="3" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2228" s="6" t="s">
-        <v>1732</v>
+        <v>1729</v>
       </c>
       <c r="G2228" s="5"/>
     </row>
     <row r="2229" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2229" s="9" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="B2229" s="7" t="s">
-        <v>1736</v>
+        <v>1733</v>
       </c>
       <c r="C2229" s="7" t="s">
         <v>35</v>
@@ -68514,19 +68496,19 @@
         <v>4</v>
       </c>
       <c r="E2229" s="7" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2229" s="7" t="s">
-        <v>1737</v>
+        <v>1734</v>
       </c>
       <c r="G2229" s="5"/>
     </row>
     <row r="2230" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2230" s="2" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="B2230" s="3" t="s">
-        <v>1736</v>
+        <v>1733</v>
       </c>
       <c r="C2230" s="3" t="s">
         <v>35</v>
@@ -68535,19 +68517,19 @@
         <v>4</v>
       </c>
       <c r="E2230" s="3" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2230" s="6" t="s">
-        <v>1738</v>
+        <v>1735</v>
       </c>
       <c r="G2230" s="5"/>
     </row>
     <row r="2231" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2231" s="9" t="s">
-        <v>1739</v>
+        <v>1736</v>
       </c>
       <c r="B2231" s="7" t="s">
-        <v>1740</v>
+        <v>1737</v>
       </c>
       <c r="C2231" s="7" t="s">
         <v>35</v>
@@ -68556,19 +68538,19 @@
         <v>4</v>
       </c>
       <c r="E2231" s="7" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2231" s="7" t="s">
-        <v>1684</v>
+        <v>1681</v>
       </c>
       <c r="G2231" s="5"/>
     </row>
     <row r="2232" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2232" s="9" t="s">
-        <v>1739</v>
+        <v>1736</v>
       </c>
       <c r="B2232" s="7" t="s">
-        <v>1740</v>
+        <v>1737</v>
       </c>
       <c r="C2232" s="7" t="s">
         <v>35</v>
@@ -68577,19 +68559,19 @@
         <v>4</v>
       </c>
       <c r="E2232" s="7" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2232" s="7" t="s">
-        <v>1741</v>
+        <v>1738</v>
       </c>
       <c r="G2232" s="5"/>
     </row>
     <row r="2233" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2233" s="2" t="s">
-        <v>1739</v>
+        <v>1736</v>
       </c>
       <c r="B2233" s="3" t="s">
-        <v>1740</v>
+        <v>1737</v>
       </c>
       <c r="C2233" s="3" t="s">
         <v>35</v>
@@ -68598,19 +68580,19 @@
         <v>4</v>
       </c>
       <c r="E2233" s="3" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2233" s="3" t="s">
-        <v>1742</v>
+        <v>1739</v>
       </c>
       <c r="G2233" s="5"/>
     </row>
     <row r="2234" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2234" s="9" t="s">
-        <v>1739</v>
+        <v>1736</v>
       </c>
       <c r="B2234" s="7" t="s">
-        <v>1740</v>
+        <v>1737</v>
       </c>
       <c r="C2234" s="7" t="s">
         <v>35</v>
@@ -68619,7 +68601,7 @@
         <v>4</v>
       </c>
       <c r="E2234" s="7" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2234" s="7" t="s">
         <v>1440</v>
@@ -68628,10 +68610,10 @@
     </row>
     <row r="2235" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2235" s="2" t="s">
-        <v>1743</v>
+        <v>1740</v>
       </c>
       <c r="B2235" s="6" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="C2235" s="3" t="s">
         <v>35</v>
@@ -68640,7 +68622,7 @@
         <v>4</v>
       </c>
       <c r="E2235" s="3" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2235" s="3" t="s">
         <v>1442</v>
@@ -68649,10 +68631,10 @@
     </row>
     <row r="2236" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2236" s="2" t="s">
-        <v>1743</v>
+        <v>1740</v>
       </c>
       <c r="B2236" s="6" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="C2236" s="3" t="s">
         <v>35</v>
@@ -68661,19 +68643,19 @@
         <v>4</v>
       </c>
       <c r="E2236" s="3" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2236" s="3" t="s">
-        <v>1722</v>
+        <v>1719</v>
       </c>
       <c r="G2236" s="5"/>
     </row>
     <row r="2237" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2237" s="2" t="s">
-        <v>1743</v>
+        <v>1740</v>
       </c>
       <c r="B2237" s="6" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="C2237" s="3" t="s">
         <v>35</v>
@@ -68682,19 +68664,19 @@
         <v>4</v>
       </c>
       <c r="E2237" s="3" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2237" s="6" t="s">
-        <v>1745</v>
+        <v>1742</v>
       </c>
       <c r="G2237" s="5"/>
     </row>
     <row r="2238" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2238" s="2" t="s">
-        <v>1743</v>
+        <v>1740</v>
       </c>
       <c r="B2238" s="6" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="C2238" s="3" t="s">
         <v>35</v>
@@ -68703,19 +68685,19 @@
         <v>4</v>
       </c>
       <c r="E2238" s="3" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2238" s="6" t="s">
-        <v>1746</v>
+        <v>1743</v>
       </c>
       <c r="G2238" s="5"/>
     </row>
     <row r="2239" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2239" s="2" t="s">
-        <v>1747</v>
+        <v>1744</v>
       </c>
       <c r="B2239" s="3" t="s">
-        <v>1748</v>
+        <v>1745</v>
       </c>
       <c r="C2239" s="3" t="s">
         <v>35</v>
@@ -68724,19 +68706,19 @@
         <v>4</v>
       </c>
       <c r="E2239" s="3" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2239" s="6" t="s">
-        <v>1732</v>
+        <v>1729</v>
       </c>
       <c r="G2239" s="5"/>
     </row>
     <row r="2240" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2240" s="2" t="s">
-        <v>1749</v>
+        <v>1746</v>
       </c>
       <c r="B2240" s="3" t="s">
-        <v>1750</v>
+        <v>1747</v>
       </c>
       <c r="C2240" s="3" t="s">
         <v>35</v>
@@ -68745,7 +68727,7 @@
         <v>4</v>
       </c>
       <c r="E2240" s="3" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2240" s="6" t="s">
         <v>1438</v>
@@ -68754,10 +68736,10 @@
     </row>
     <row r="2241" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2241" s="2" t="s">
-        <v>1751</v>
+        <v>1748</v>
       </c>
       <c r="B2241" s="3" t="s">
-        <v>1752</v>
+        <v>1749</v>
       </c>
       <c r="C2241" s="3" t="s">
         <v>35</v>
@@ -68766,19 +68748,19 @@
         <v>4</v>
       </c>
       <c r="E2241" s="3" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2241" s="6" t="s">
-        <v>1753</v>
+        <v>1750</v>
       </c>
       <c r="G2241" s="5"/>
     </row>
     <row r="2242" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2242" s="2" t="s">
-        <v>1754</v>
+        <v>1751</v>
       </c>
       <c r="B2242" s="3" t="s">
-        <v>1755</v>
+        <v>1752</v>
       </c>
       <c r="C2242" s="3" t="s">
         <v>35</v>
@@ -68787,19 +68769,19 @@
         <v>4</v>
       </c>
       <c r="E2242" s="3" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2242" s="3" t="s">
-        <v>1714</v>
+        <v>1711</v>
       </c>
       <c r="G2242" s="5"/>
     </row>
     <row r="2243" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2243" s="9" t="s">
-        <v>1756</v>
+        <v>1753</v>
       </c>
       <c r="B2243" s="7" t="s">
-        <v>1757</v>
+        <v>1754</v>
       </c>
       <c r="C2243" s="7" t="s">
         <v>35</v>
@@ -68808,19 +68790,19 @@
         <v>4</v>
       </c>
       <c r="E2243" s="7" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2243" s="7" t="s">
-        <v>1727</v>
+        <v>1724</v>
       </c>
       <c r="G2243" s="5"/>
     </row>
     <row r="2244" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2244" s="9" t="s">
-        <v>1758</v>
+        <v>1755</v>
       </c>
       <c r="B2244" s="7" t="s">
-        <v>1759</v>
+        <v>1756</v>
       </c>
       <c r="C2244" s="7" t="s">
         <v>35</v>
@@ -68829,19 +68811,19 @@
         <v>4</v>
       </c>
       <c r="E2244" s="7" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2244" s="7" t="s">
-        <v>1760</v>
+        <v>1757</v>
       </c>
       <c r="G2244" s="5"/>
     </row>
     <row r="2245" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2245" s="2" t="s">
-        <v>1761</v>
+        <v>1758</v>
       </c>
       <c r="B2245" s="3" t="s">
-        <v>1762</v>
+        <v>1759</v>
       </c>
       <c r="C2245" s="3" t="s">
         <v>35</v>
@@ -68850,19 +68832,19 @@
         <v>4</v>
       </c>
       <c r="E2245" s="3" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2245" s="3" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="G2245" s="5"/>
     </row>
     <row r="2246" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2246" s="2" t="s">
-        <v>1763</v>
+        <v>1760</v>
       </c>
       <c r="B2246" s="6" t="s">
-        <v>1764</v>
+        <v>1761</v>
       </c>
       <c r="C2246" s="3" t="s">
         <v>35</v>
@@ -68871,19 +68853,19 @@
         <v>4</v>
       </c>
       <c r="E2246" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2246" s="3" t="s">
-        <v>1765</v>
+        <v>1762</v>
       </c>
       <c r="G2246" s="5"/>
     </row>
     <row r="2247" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2247" s="2" t="s">
-        <v>1766</v>
+        <v>1763</v>
       </c>
       <c r="B2247" s="3" t="s">
-        <v>1767</v>
+        <v>1764</v>
       </c>
       <c r="C2247" s="3" t="s">
         <v>35</v>
@@ -68892,19 +68874,19 @@
         <v>4</v>
       </c>
       <c r="E2247" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2247" s="3" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
       <c r="G2247" s="5"/>
     </row>
     <row r="2248" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2248" s="2" t="s">
-        <v>1768</v>
+        <v>1765</v>
       </c>
       <c r="B2248" s="6" t="s">
-        <v>1769</v>
+        <v>1766</v>
       </c>
       <c r="C2248" s="3" t="s">
         <v>35</v>
@@ -68913,19 +68895,19 @@
         <v>4</v>
       </c>
       <c r="E2248" s="3" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
       <c r="F2248" s="6" t="s">
-        <v>1770</v>
+        <v>1767</v>
       </c>
       <c r="G2248" s="5"/>
     </row>
     <row r="2249" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2249" s="9" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
       <c r="B2249" s="7" t="s">
-        <v>1772</v>
+        <v>1769</v>
       </c>
       <c r="C2249" s="7" t="s">
         <v>35</v>
@@ -68934,19 +68916,19 @@
         <v>4</v>
       </c>
       <c r="E2249" s="7" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2249" s="7" t="s">
-        <v>1707</v>
+        <v>1704</v>
       </c>
       <c r="G2249" s="5"/>
     </row>
     <row r="2250" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2250" s="9" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
       <c r="B2250" s="7" t="s">
-        <v>1772</v>
+        <v>1769</v>
       </c>
       <c r="C2250" s="7" t="s">
         <v>35</v>
@@ -68955,19 +68937,19 @@
         <v>4</v>
       </c>
       <c r="E2250" s="7" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2250" s="7" t="s">
-        <v>1773</v>
+        <v>1770</v>
       </c>
       <c r="G2250" s="5"/>
     </row>
     <row r="2251" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2251" s="9" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
       <c r="B2251" s="7" t="s">
-        <v>1772</v>
+        <v>1769</v>
       </c>
       <c r="C2251" s="7" t="s">
         <v>35</v>
@@ -68976,19 +68958,19 @@
         <v>4</v>
       </c>
       <c r="E2251" s="7" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2251" s="7" t="s">
-        <v>1722</v>
+        <v>1719</v>
       </c>
       <c r="G2251" s="5"/>
     </row>
     <row r="2252" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2252" s="2" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
       <c r="B2252" s="3" t="s">
-        <v>1772</v>
+        <v>1769</v>
       </c>
       <c r="C2252" s="3" t="s">
         <v>35</v>
@@ -68997,19 +68979,19 @@
         <v>4</v>
       </c>
       <c r="E2252" s="3" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2252" s="3" t="s">
-        <v>1742</v>
+        <v>1739</v>
       </c>
       <c r="G2252" s="5"/>
     </row>
     <row r="2253" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2253" s="2" t="s">
-        <v>1774</v>
+        <v>1771</v>
       </c>
       <c r="B2253" s="6" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
       <c r="C2253" s="3" t="s">
         <v>35</v>
@@ -69018,19 +69000,19 @@
         <v>4</v>
       </c>
       <c r="E2253" s="3" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2253" s="6" t="s">
-        <v>1776</v>
+        <v>1773</v>
       </c>
       <c r="G2253" s="5"/>
     </row>
     <row r="2254" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2254" s="2" t="s">
-        <v>1774</v>
+        <v>1771</v>
       </c>
       <c r="B2254" s="6" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
       <c r="C2254" s="3" t="s">
         <v>35</v>
@@ -69039,7 +69021,7 @@
         <v>4</v>
       </c>
       <c r="E2254" s="3" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2254" s="3" t="s">
         <v>1435</v>
@@ -69048,10 +69030,10 @@
     </row>
     <row r="2255" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2255" s="2" t="s">
-        <v>1777</v>
+        <v>1774</v>
       </c>
       <c r="B2255" s="6" t="s">
-        <v>1778</v>
+        <v>1775</v>
       </c>
       <c r="C2255" s="3" t="s">
         <v>35</v>
@@ -69060,19 +69042,19 @@
         <v>4</v>
       </c>
       <c r="E2255" s="3" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2255" s="3" t="s">
-        <v>1779</v>
+        <v>1776</v>
       </c>
       <c r="G2255" s="5"/>
     </row>
     <row r="2256" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2256" s="2" t="s">
-        <v>1777</v>
+        <v>1774</v>
       </c>
       <c r="B2256" s="6" t="s">
-        <v>1778</v>
+        <v>1775</v>
       </c>
       <c r="C2256" s="3" t="s">
         <v>35</v>
@@ -69081,19 +69063,19 @@
         <v>4</v>
       </c>
       <c r="E2256" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2256" s="3" t="s">
-        <v>1779</v>
+        <v>1776</v>
       </c>
       <c r="G2256" s="5"/>
     </row>
     <row r="2257" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2257" s="2" t="s">
-        <v>1780</v>
+        <v>1777</v>
       </c>
       <c r="B2257" s="3" t="s">
-        <v>1781</v>
+        <v>1778</v>
       </c>
       <c r="C2257" s="3" t="s">
         <v>35</v>
@@ -69102,19 +69084,19 @@
         <v>4</v>
       </c>
       <c r="E2257" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2257" s="3" t="s">
-        <v>1782</v>
+        <v>1779</v>
       </c>
       <c r="G2257" s="5"/>
     </row>
     <row r="2258" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2258" s="2" t="s">
-        <v>1780</v>
+        <v>1777</v>
       </c>
       <c r="B2258" s="3" t="s">
-        <v>1781</v>
+        <v>1778</v>
       </c>
       <c r="C2258" s="3" t="s">
         <v>35</v>
@@ -69123,19 +69105,19 @@
         <v>4</v>
       </c>
       <c r="E2258" s="3" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2258" s="3" t="s">
-        <v>1783</v>
+        <v>1780</v>
       </c>
       <c r="G2258" s="5"/>
     </row>
     <row r="2259" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2259" s="2" t="s">
-        <v>1784</v>
+        <v>1781</v>
       </c>
       <c r="B2259" s="3" t="s">
-        <v>1785</v>
+        <v>1782</v>
       </c>
       <c r="C2259" s="3" t="s">
         <v>35</v>
@@ -69144,7 +69126,7 @@
         <v>4</v>
       </c>
       <c r="E2259" s="3" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2259" s="6" t="s">
         <v>1241</v>
@@ -69153,10 +69135,10 @@
     </row>
     <row r="2260" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2260" s="9" t="s">
-        <v>1784</v>
+        <v>1781</v>
       </c>
       <c r="B2260" s="7" t="s">
-        <v>1785</v>
+        <v>1782</v>
       </c>
       <c r="C2260" s="7" t="s">
         <v>35</v>
@@ -69165,7 +69147,7 @@
         <v>4</v>
       </c>
       <c r="E2260" s="7" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2260" s="7" t="s">
         <v>780</v>
@@ -69174,10 +69156,10 @@
     </row>
     <row r="2261" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2261" s="2" t="s">
-        <v>1786</v>
+        <v>1783</v>
       </c>
       <c r="B2261" s="3" t="s">
-        <v>1575</v>
+        <v>1572</v>
       </c>
       <c r="C2261" s="3" t="s">
         <v>35</v>
@@ -69186,7 +69168,7 @@
         <v>4</v>
       </c>
       <c r="E2261" s="3" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2261" s="6" t="s">
         <v>1418</v>
@@ -69195,10 +69177,10 @@
     </row>
     <row r="2262" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2262" s="2" t="s">
-        <v>1786</v>
+        <v>1783</v>
       </c>
       <c r="B2262" s="3" t="s">
-        <v>1575</v>
+        <v>1572</v>
       </c>
       <c r="C2262" s="3" t="s">
         <v>35</v>
@@ -69207,19 +69189,19 @@
         <v>4</v>
       </c>
       <c r="E2262" s="3" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2262" s="7" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
       <c r="G2262" s="5"/>
     </row>
     <row r="2263" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2263" s="2" t="s">
-        <v>1787</v>
+        <v>1784</v>
       </c>
       <c r="B2263" s="3" t="s">
-        <v>1532</v>
+        <v>1529</v>
       </c>
       <c r="C2263" s="3" t="s">
         <v>35</v>
@@ -69228,19 +69210,19 @@
         <v>4</v>
       </c>
       <c r="E2263" s="3" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="F2263" s="6" t="s">
-        <v>1788</v>
+        <v>1785</v>
       </c>
       <c r="G2263" s="5"/>
     </row>
     <row r="2264" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2264" s="2" t="s">
-        <v>1787</v>
+        <v>1784</v>
       </c>
       <c r="B2264" s="3" t="s">
-        <v>1532</v>
+        <v>1529</v>
       </c>
       <c r="C2264" s="3" t="s">
         <v>35</v>
@@ -69249,19 +69231,19 @@
         <v>4</v>
       </c>
       <c r="E2264" s="3" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2264" s="6" t="s">
-        <v>1788</v>
+        <v>1785</v>
       </c>
       <c r="G2264" s="5"/>
     </row>
     <row r="2265" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2265" s="2" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="B2265" s="3" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="C2265" s="3" t="s">
         <v>150</v>
@@ -69270,7 +69252,7 @@
         <v>3</v>
       </c>
       <c r="E2265" s="3" t="s">
-        <v>1791</v>
+        <v>1788</v>
       </c>
       <c r="F2265" s="6" t="s">
         <v>1439</v>
@@ -69279,10 +69261,10 @@
     </row>
     <row r="2266" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2266" s="9" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="B2266" s="7" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="C2266" s="7" t="s">
         <v>150</v>
@@ -69291,19 +69273,19 @@
         <v>3</v>
       </c>
       <c r="E2266" s="7" t="s">
-        <v>1791</v>
+        <v>1788</v>
       </c>
       <c r="F2266" s="7" t="s">
-        <v>1692</v>
+        <v>1689</v>
       </c>
       <c r="G2266" s="5"/>
     </row>
     <row r="2267" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2267" s="9" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="B2267" s="7" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="C2267" s="7" t="s">
         <v>150</v>
@@ -69312,7 +69294,7 @@
         <v>3</v>
       </c>
       <c r="E2267" s="7" t="s">
-        <v>1791</v>
+        <v>1788</v>
       </c>
       <c r="F2267" s="7" t="s">
         <v>1441</v>
@@ -69321,10 +69303,10 @@
     </row>
     <row r="2268" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2268" s="2" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="B2268" s="3" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="C2268" s="3" t="s">
         <v>150</v>
@@ -69333,19 +69315,19 @@
         <v>3</v>
       </c>
       <c r="E2268" s="3" t="s">
-        <v>1791</v>
+        <v>1788</v>
       </c>
       <c r="F2268" s="6" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="G2268" s="5"/>
     </row>
     <row r="2269" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2269" s="2" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="B2269" s="3" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="C2269" s="3" t="s">
         <v>152</v>
@@ -69354,7 +69336,7 @@
         <v>1</v>
       </c>
       <c r="E2269" s="3" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="F2269" s="6" t="s">
         <v>1439</v>
@@ -69363,10 +69345,10 @@
     </row>
     <row r="2270" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2270" s="9" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="B2270" s="7" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="C2270" s="7" t="s">
         <v>152</v>
@@ -69375,19 +69357,19 @@
         <v>1</v>
       </c>
       <c r="E2270" s="7" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="F2270" s="7" t="s">
-        <v>1692</v>
+        <v>1689</v>
       </c>
       <c r="G2270" s="5"/>
     </row>
     <row r="2271" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2271" s="9" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="B2271" s="7" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="C2271" s="7" t="s">
         <v>152</v>
@@ -69396,7 +69378,7 @@
         <v>1</v>
       </c>
       <c r="E2271" s="7" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="F2271" s="7" t="s">
         <v>1441</v>
@@ -69405,10 +69387,10 @@
     </row>
     <row r="2272" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2272" s="2" t="s">
-        <v>1789</v>
+        <v>1786</v>
       </c>
       <c r="B2272" s="3" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
       <c r="C2272" s="3" t="s">
         <v>152</v>
@@ -69417,19 +69399,19 @@
         <v>1</v>
       </c>
       <c r="E2272" s="3" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="F2272" s="6" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
       <c r="G2272" s="5"/>
     </row>
     <row r="2273" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2273" s="9" t="s">
-        <v>1793</v>
+        <v>1790</v>
       </c>
       <c r="B2273" s="7" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
       <c r="C2273" s="7" t="s">
         <v>35</v>
@@ -69438,19 +69420,19 @@
         <v>4</v>
       </c>
       <c r="E2273" s="7" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2273" s="7" t="s">
-        <v>1795</v>
+        <v>1792</v>
       </c>
       <c r="G2273" s="5"/>
     </row>
     <row r="2274" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2274" s="9" t="s">
-        <v>1793</v>
+        <v>1790</v>
       </c>
       <c r="B2274" s="7" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
       <c r="C2274" s="7" t="s">
         <v>35</v>
@@ -69459,19 +69441,19 @@
         <v>4</v>
       </c>
       <c r="E2274" s="7" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2274" s="7" t="s">
-        <v>1728</v>
+        <v>1725</v>
       </c>
       <c r="G2274" s="5"/>
     </row>
     <row r="2275" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2275" s="9" t="s">
-        <v>1793</v>
+        <v>1790</v>
       </c>
       <c r="B2275" s="7" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
       <c r="C2275" s="7" t="s">
         <v>35</v>
@@ -69480,19 +69462,19 @@
         <v>4</v>
       </c>
       <c r="E2275" s="7" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2275" s="7" t="s">
-        <v>1695</v>
+        <v>1692</v>
       </c>
       <c r="G2275" s="5"/>
     </row>
     <row r="2276" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2276" s="9" t="s">
-        <v>1793</v>
+        <v>1790</v>
       </c>
       <c r="B2276" s="7" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
       <c r="C2276" s="7" t="s">
         <v>35</v>
@@ -69501,7 +69483,7 @@
         <v>4</v>
       </c>
       <c r="E2276" s="7" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="F2276" s="7" t="s">
         <v>1271</v>
@@ -69510,10 +69492,10 @@
     </row>
     <row r="2277" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2277" s="9" t="s">
-        <v>1796</v>
+        <v>1793</v>
       </c>
       <c r="B2277" s="7" t="s">
-        <v>1797</v>
+        <v>1794</v>
       </c>
       <c r="C2277" s="7" t="s">
         <v>35</v>
@@ -69522,7 +69504,7 @@
         <v>4</v>
       </c>
       <c r="E2277" s="7" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2277" s="7" t="s">
         <v>1440</v>
@@ -69531,10 +69513,10 @@
     </row>
     <row r="2278" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2278" s="9" t="s">
-        <v>1796</v>
+        <v>1793</v>
       </c>
       <c r="B2278" s="7" t="s">
-        <v>1797</v>
+        <v>1794</v>
       </c>
       <c r="C2278" s="7" t="s">
         <v>35</v>
@@ -69543,19 +69525,19 @@
         <v>4</v>
       </c>
       <c r="E2278" s="7" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2278" s="7" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="G2278" s="5"/>
     </row>
     <row r="2279" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2279" s="9" t="s">
-        <v>1796</v>
+        <v>1793</v>
       </c>
       <c r="B2279" s="7" t="s">
-        <v>1797</v>
+        <v>1794</v>
       </c>
       <c r="C2279" s="7" t="s">
         <v>35</v>
@@ -69564,7 +69546,7 @@
         <v>4</v>
       </c>
       <c r="E2279" s="7" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2279" s="7" t="s">
         <v>1442</v>
@@ -69573,10 +69555,10 @@
     </row>
     <row r="2280" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2280" s="2" t="s">
-        <v>1796</v>
+        <v>1793</v>
       </c>
       <c r="B2280" s="3" t="s">
-        <v>1797</v>
+        <v>1794</v>
       </c>
       <c r="C2280" s="3" t="s">
         <v>35</v>
@@ -69585,19 +69567,19 @@
         <v>4</v>
       </c>
       <c r="E2280" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2280" s="3" t="s">
-        <v>1714</v>
+        <v>1711</v>
       </c>
       <c r="G2280" s="5"/>
     </row>
     <row r="2281" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2281" s="2" t="s">
-        <v>1798</v>
+        <v>1795</v>
       </c>
       <c r="B2281" s="6" t="s">
-        <v>1799</v>
+        <v>1796</v>
       </c>
       <c r="C2281" s="3" t="s">
         <v>35</v>
@@ -69606,19 +69588,19 @@
         <v>4</v>
       </c>
       <c r="E2281" s="3" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2281" s="3" t="s">
-        <v>1742</v>
+        <v>1739</v>
       </c>
       <c r="G2281" s="5"/>
     </row>
     <row r="2282" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2282" s="2" t="s">
-        <v>1798</v>
+        <v>1795</v>
       </c>
       <c r="B2282" s="6" t="s">
-        <v>1799</v>
+        <v>1796</v>
       </c>
       <c r="C2282" s="3" t="s">
         <v>35</v>
@@ -69627,19 +69609,19 @@
         <v>4</v>
       </c>
       <c r="E2282" s="3" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2282" s="3" t="s">
-        <v>1729</v>
+        <v>1726</v>
       </c>
       <c r="G2282" s="5"/>
     </row>
     <row r="2283" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2283" s="2" t="s">
-        <v>1798</v>
+        <v>1795</v>
       </c>
       <c r="B2283" s="6" t="s">
-        <v>1799</v>
+        <v>1796</v>
       </c>
       <c r="C2283" s="3" t="s">
         <v>35</v>
@@ -69648,19 +69630,19 @@
         <v>4</v>
       </c>
       <c r="E2283" s="3" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2283" s="6" t="s">
-        <v>1745</v>
+        <v>1742</v>
       </c>
       <c r="G2283" s="5"/>
     </row>
     <row r="2284" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2284" s="2" t="s">
-        <v>1798</v>
+        <v>1795</v>
       </c>
       <c r="B2284" s="6" t="s">
-        <v>1799</v>
+        <v>1796</v>
       </c>
       <c r="C2284" s="3" t="s">
         <v>35</v>
@@ -69669,19 +69651,19 @@
         <v>4</v>
       </c>
       <c r="E2284" s="3" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="F2284" s="3" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="G2284" s="5"/>
     </row>
     <row r="2285" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2285" s="2" t="s">
-        <v>1800</v>
+        <v>1797</v>
       </c>
       <c r="B2285" s="3" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
       <c r="C2285" s="3" t="s">
         <v>35</v>
@@ -69690,19 +69672,19 @@
         <v>4</v>
       </c>
       <c r="E2285" s="3" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2285" s="6" t="s">
-        <v>1776</v>
+        <v>1773</v>
       </c>
       <c r="G2285" s="5"/>
     </row>
     <row r="2286" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2286" s="9" t="s">
-        <v>1800</v>
+        <v>1797</v>
       </c>
       <c r="B2286" s="7" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
       <c r="C2286" s="7" t="s">
         <v>35</v>
@@ -69711,7 +69693,7 @@
         <v>4</v>
       </c>
       <c r="E2286" s="7" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="F2286" s="7" t="s">
         <v>1435</v>
@@ -69720,10 +69702,10 @@
     </row>
     <row r="2287" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2287" s="2" t="s">
-        <v>1802</v>
+        <v>1799</v>
       </c>
       <c r="B2287" s="6" t="s">
-        <v>1803</v>
+        <v>1800</v>
       </c>
       <c r="C2287" s="3" t="s">
         <v>35</v>
@@ -69732,19 +69714,19 @@
         <v>4</v>
       </c>
       <c r="E2287" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2287" s="6" t="s">
-        <v>1804</v>
+        <v>1801</v>
       </c>
       <c r="G2287" s="5"/>
     </row>
     <row r="2288" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2288" s="2" t="s">
-        <v>1802</v>
+        <v>1799</v>
       </c>
       <c r="B2288" s="6" t="s">
-        <v>1803</v>
+        <v>1800</v>
       </c>
       <c r="C2288" s="3" t="s">
         <v>35</v>
@@ -69753,10 +69735,10 @@
         <v>4</v>
       </c>
       <c r="E2288" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="F2288" s="3" t="s">
-        <v>1805</v>
+        <v>1802</v>
       </c>
       <c r="G2288" s="5"/>
     </row>

</xml_diff>